<commit_message>
Bootloader Working still and config good
This is a good place to continue the configure
</commit_message>
<xml_diff>
--- a/Wifi bootloader prelim CPD 5.xlsx
+++ b/Wifi bootloader prelim CPD 5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\Booyco HMI Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA76785-FDDB-406B-A61C-A55F2D2FDC12}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CC569D-D49F-4572-AD90-E86263F916FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="840" windowWidth="24840" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="85">
   <si>
     <t>SOF1</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>Acknowledgement from device that it is ready to send</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -627,11 +633,11 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Explanatory Text" xfId="6" builtinId="53"/>
@@ -952,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,22 +1003,22 @@
       <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
@@ -1926,7 +1932,7 @@
       <c r="AF17" s="8"/>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="27" t="s">
         <v>80</v>
       </c>
       <c r="B18" s="2">
@@ -1959,7 +1965,7 @@
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="2">
@@ -1992,7 +1998,7 @@
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="27" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="2">
@@ -2090,7 +2096,7 @@
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="2">
@@ -2132,7 +2138,7 @@
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="27" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="2">
@@ -2171,7 +2177,7 @@
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="27" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="2">
@@ -2204,7 +2210,7 @@
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="28" t="s">
         <v>81</v>
       </c>
       <c r="B25" s="2">
@@ -2237,11 +2243,11 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="28" t="s">
         <v>82</v>
       </c>
       <c r="B26" s="2">
-        <f t="shared" ref="B26:B30" si="1">COUNTA(C26:I26)</f>
+        <f t="shared" ref="B26" si="1">COUNTA(C26:I26)</f>
         <v>7</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -2270,7 +2276,7 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="2">
@@ -2368,7 +2374,7 @@
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2">
@@ -2410,7 +2416,7 @@
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="2">
@@ -2449,11 +2455,11 @@
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="2">
-        <f t="shared" si="2"/>
+        <f>COUNTA(C28:I28)</f>
         <v>7</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -2479,6 +2485,66 @@
       </c>
       <c r="J30" s="4" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <f>COUNTA(C30:I30)</f>
+        <v>7</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <f>COUNTA(C31:I31)</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>